<commit_message>
Add LaTeX table producer function; update Readme
</commit_message>
<xml_diff>
--- a/output/summary.xlsx
+++ b/output/summary.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Transaction Cost</t>
   </si>
@@ -26,16 +26,16 @@
     <t>Total Return</t>
   </si>
   <si>
-    <t>Annualised Return</t>
+    <t>Return (Ann.)</t>
   </si>
   <si>
     <t>Sharpe Ratio</t>
   </si>
   <si>
-    <t>Sharpe Ratio (Ann)</t>
+    <t>Sharpe Ratio (Ann.)</t>
   </si>
   <si>
-    <t>Volatility</t>
+    <t>Volatility (Ann.)</t>
   </si>
   <si>
     <t>Max Drawdown</t>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Longest Drawdown (Days)</t>
+  </si>
+  <si>
+    <t>2003-08-05</t>
   </si>
   <si>
     <t>NAV</t>
@@ -116,13 +119,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -466,31 +468,31 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>0.015</v>
       </c>
       <c r="C2" s="1">
-        <v>0.1038105000000007</v>
+        <v>0.1039192000000007</v>
       </c>
       <c r="D2" s="1">
-        <v>0.07220662267557376</v>
+        <v>0.07228115412102953</v>
       </c>
       <c r="E2">
-        <v>1.161593006811779</v>
+        <v>0.9229974308412767</v>
       </c>
       <c r="F2">
-        <v>0.9773030635770681</v>
+        <v>0.7765613356357848</v>
       </c>
       <c r="G2" s="1">
-        <v>0.08839460052926004</v>
+        <v>0.07436912627128299</v>
       </c>
       <c r="H2" s="1">
         <v>0.044239754036693</v>
       </c>
-      <c r="I2" s="3">
-        <v>37838</v>
+      <c r="I2" t="s">
+        <v>10</v>
       </c>
       <c r="J2">
         <v>107</v>
@@ -514,17 +516,17 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>37804</v>
       </c>
       <c r="B2">
@@ -538,7 +540,7 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>37805</v>
       </c>
       <c r="B3">
@@ -552,7 +554,7 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>37806</v>
       </c>
       <c r="B4">
@@ -566,7 +568,7 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>37807</v>
       </c>
       <c r="B5">
@@ -580,7 +582,7 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>37808</v>
       </c>
       <c r="B6">
@@ -594,7 +596,7 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>37809</v>
       </c>
       <c r="B7">
@@ -608,7 +610,7 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>37810</v>
       </c>
       <c r="B8">
@@ -622,7 +624,7 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>37811</v>
       </c>
       <c r="B9">
@@ -636,7 +638,7 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>37812</v>
       </c>
       <c r="B10">
@@ -650,7 +652,7 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>37813</v>
       </c>
       <c r="B11">
@@ -664,7 +666,7 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>37814</v>
       </c>
       <c r="B12">
@@ -678,7 +680,7 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>37815</v>
       </c>
       <c r="B13">
@@ -692,7 +694,7 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>37816</v>
       </c>
       <c r="B14">
@@ -706,7 +708,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>37817</v>
       </c>
       <c r="B15">
@@ -720,7 +722,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>37818</v>
       </c>
       <c r="B16">
@@ -734,7 +736,7 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>37819</v>
       </c>
       <c r="B17">
@@ -748,7 +750,7 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>37820</v>
       </c>
       <c r="B18">
@@ -762,7 +764,7 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>37821</v>
       </c>
       <c r="B19">
@@ -776,7 +778,7 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>37822</v>
       </c>
       <c r="B20">
@@ -790,7 +792,7 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>37823</v>
       </c>
       <c r="B21">
@@ -804,7 +806,7 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>37824</v>
       </c>
       <c r="B22">
@@ -818,7 +820,7 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>37825</v>
       </c>
       <c r="B23">
@@ -832,7 +834,7 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>37826</v>
       </c>
       <c r="B24">
@@ -846,7 +848,7 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>37827</v>
       </c>
       <c r="B25">
@@ -860,7 +862,7 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>37828</v>
       </c>
       <c r="B26">
@@ -874,7 +876,7 @@
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>37829</v>
       </c>
       <c r="B27">
@@ -888,7 +890,7 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>37830</v>
       </c>
       <c r="B28">
@@ -902,7 +904,7 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>37831</v>
       </c>
       <c r="B29">
@@ -916,7 +918,7 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>37832</v>
       </c>
       <c r="B30">
@@ -930,7 +932,7 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>37833</v>
       </c>
       <c r="B31">
@@ -944,7 +946,7 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>37834</v>
       </c>
       <c r="B32">
@@ -958,7 +960,7 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>37835</v>
       </c>
       <c r="B33">
@@ -972,7 +974,7 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>37836</v>
       </c>
       <c r="B34">
@@ -986,7 +988,7 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>37837</v>
       </c>
       <c r="B35">
@@ -1000,7 +1002,7 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>37838</v>
       </c>
       <c r="B36">
@@ -1014,7 +1016,7 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>37839</v>
       </c>
       <c r="B37">
@@ -1028,7 +1030,7 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>37840</v>
       </c>
       <c r="B38">
@@ -1042,7 +1044,7 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>37841</v>
       </c>
       <c r="B39">
@@ -1056,7 +1058,7 @@
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>37842</v>
       </c>
       <c r="B40">
@@ -1070,7 +1072,7 @@
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>37843</v>
       </c>
       <c r="B41">
@@ -1084,7 +1086,7 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>37844</v>
       </c>
       <c r="B42">
@@ -1098,7 +1100,7 @@
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>37845</v>
       </c>
       <c r="B43">
@@ -1112,7 +1114,7 @@
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>37846</v>
       </c>
       <c r="B44">
@@ -1126,7 +1128,7 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>37847</v>
       </c>
       <c r="B45">
@@ -1140,7 +1142,7 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>37848</v>
       </c>
       <c r="B46">
@@ -1154,7 +1156,7 @@
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>37849</v>
       </c>
       <c r="B47">
@@ -1168,7 +1170,7 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>37850</v>
       </c>
       <c r="B48">
@@ -1182,7 +1184,7 @@
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>37851</v>
       </c>
       <c r="B49">
@@ -1196,7 +1198,7 @@
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="4">
+      <c r="A50" s="3">
         <v>37852</v>
       </c>
       <c r="B50">
@@ -1210,7 +1212,7 @@
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>37853</v>
       </c>
       <c r="B51">
@@ -1224,7 +1226,7 @@
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>37854</v>
       </c>
       <c r="B52">
@@ -1238,7 +1240,7 @@
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>37855</v>
       </c>
       <c r="B53">
@@ -1252,7 +1254,7 @@
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>37856</v>
       </c>
       <c r="B54">
@@ -1266,7 +1268,7 @@
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>37857</v>
       </c>
       <c r="B55">
@@ -1280,7 +1282,7 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>37858</v>
       </c>
       <c r="B56">
@@ -1294,7 +1296,7 @@
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="4">
+      <c r="A57" s="3">
         <v>37859</v>
       </c>
       <c r="B57">
@@ -1308,7 +1310,7 @@
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>37860</v>
       </c>
       <c r="B58">
@@ -1322,7 +1324,7 @@
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="4">
+      <c r="A59" s="3">
         <v>37861</v>
       </c>
       <c r="B59">
@@ -1336,7 +1338,7 @@
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="4">
+      <c r="A60" s="3">
         <v>37862</v>
       </c>
       <c r="B60">
@@ -1350,7 +1352,7 @@
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="4">
+      <c r="A61" s="3">
         <v>37863</v>
       </c>
       <c r="B61">
@@ -1364,7 +1366,7 @@
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>37864</v>
       </c>
       <c r="B62">
@@ -1378,7 +1380,7 @@
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="4">
+      <c r="A63" s="3">
         <v>37865</v>
       </c>
       <c r="B63">
@@ -1392,7 +1394,7 @@
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="4">
+      <c r="A64" s="3">
         <v>37866</v>
       </c>
       <c r="B64">
@@ -1406,7 +1408,7 @@
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="4">
+      <c r="A65" s="3">
         <v>37867</v>
       </c>
       <c r="B65">
@@ -1420,7 +1422,7 @@
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="4">
+      <c r="A66" s="3">
         <v>37868</v>
       </c>
       <c r="B66">
@@ -1434,7 +1436,7 @@
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="4">
+      <c r="A67" s="3">
         <v>37869</v>
       </c>
       <c r="B67">
@@ -1448,7 +1450,7 @@
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="4">
+      <c r="A68" s="3">
         <v>37870</v>
       </c>
       <c r="B68">
@@ -1462,7 +1464,7 @@
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="4">
+      <c r="A69" s="3">
         <v>37871</v>
       </c>
       <c r="B69">
@@ -1476,7 +1478,7 @@
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="4">
+      <c r="A70" s="3">
         <v>37872</v>
       </c>
       <c r="B70">
@@ -1490,7 +1492,7 @@
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="4">
+      <c r="A71" s="3">
         <v>37873</v>
       </c>
       <c r="B71">
@@ -1504,7 +1506,7 @@
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="4">
+      <c r="A72" s="3">
         <v>37874</v>
       </c>
       <c r="B72">
@@ -1518,7 +1520,7 @@
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="4">
+      <c r="A73" s="3">
         <v>37875</v>
       </c>
       <c r="B73">
@@ -1532,7 +1534,7 @@
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="4">
+      <c r="A74" s="3">
         <v>37876</v>
       </c>
       <c r="B74">
@@ -1546,7 +1548,7 @@
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="4">
+      <c r="A75" s="3">
         <v>37877</v>
       </c>
       <c r="B75">
@@ -1560,7 +1562,7 @@
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="4">
+      <c r="A76" s="3">
         <v>37878</v>
       </c>
       <c r="B76">
@@ -1574,7 +1576,7 @@
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="4">
+      <c r="A77" s="3">
         <v>37879</v>
       </c>
       <c r="B77">
@@ -1588,7 +1590,7 @@
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="4">
+      <c r="A78" s="3">
         <v>37880</v>
       </c>
       <c r="B78">
@@ -1602,7 +1604,7 @@
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="4">
+      <c r="A79" s="3">
         <v>37881</v>
       </c>
       <c r="B79">
@@ -1616,7 +1618,7 @@
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="4">
+      <c r="A80" s="3">
         <v>37882</v>
       </c>
       <c r="B80">
@@ -1630,7 +1632,7 @@
       </c>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="4">
+      <c r="A81" s="3">
         <v>37883</v>
       </c>
       <c r="B81">
@@ -1644,7 +1646,7 @@
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="4">
+      <c r="A82" s="3">
         <v>37884</v>
       </c>
       <c r="B82">
@@ -1658,7 +1660,7 @@
       </c>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="4">
+      <c r="A83" s="3">
         <v>37885</v>
       </c>
       <c r="B83">
@@ -1672,7 +1674,7 @@
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="4">
+      <c r="A84" s="3">
         <v>37886</v>
       </c>
       <c r="B84">
@@ -1686,7 +1688,7 @@
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="4">
+      <c r="A85" s="3">
         <v>37887</v>
       </c>
       <c r="B85">
@@ -1700,7 +1702,7 @@
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="4">
+      <c r="A86" s="3">
         <v>37888</v>
       </c>
       <c r="B86">
@@ -1714,7 +1716,7 @@
       </c>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="4">
+      <c r="A87" s="3">
         <v>37889</v>
       </c>
       <c r="B87">
@@ -1728,7 +1730,7 @@
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="4">
+      <c r="A88" s="3">
         <v>37890</v>
       </c>
       <c r="B88">
@@ -1742,7 +1744,7 @@
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="4">
+      <c r="A89" s="3">
         <v>37891</v>
       </c>
       <c r="B89">
@@ -1756,7 +1758,7 @@
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="4">
+      <c r="A90" s="3">
         <v>37892</v>
       </c>
       <c r="B90">
@@ -1770,7 +1772,7 @@
       </c>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="4">
+      <c r="A91" s="3">
         <v>37893</v>
       </c>
       <c r="B91">
@@ -1784,7 +1786,7 @@
       </c>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="4">
+      <c r="A92" s="3">
         <v>37894</v>
       </c>
       <c r="B92">
@@ -1798,7 +1800,7 @@
       </c>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="4">
+      <c r="A93" s="3">
         <v>37895</v>
       </c>
       <c r="B93">
@@ -1812,7 +1814,7 @@
       </c>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="4">
+      <c r="A94" s="3">
         <v>37896</v>
       </c>
       <c r="B94">
@@ -1826,7 +1828,7 @@
       </c>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="4">
+      <c r="A95" s="3">
         <v>37897</v>
       </c>
       <c r="B95">
@@ -1840,7 +1842,7 @@
       </c>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="4">
+      <c r="A96" s="3">
         <v>37898</v>
       </c>
       <c r="B96">
@@ -1854,7 +1856,7 @@
       </c>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="4">
+      <c r="A97" s="3">
         <v>37899</v>
       </c>
       <c r="B97">
@@ -1868,7 +1870,7 @@
       </c>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="4">
+      <c r="A98" s="3">
         <v>37900</v>
       </c>
       <c r="B98">
@@ -1882,7 +1884,7 @@
       </c>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="4">
+      <c r="A99" s="3">
         <v>37901</v>
       </c>
       <c r="B99">
@@ -1896,7 +1898,7 @@
       </c>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="4">
+      <c r="A100" s="3">
         <v>37902</v>
       </c>
       <c r="B100">
@@ -1910,7 +1912,7 @@
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="4">
+      <c r="A101" s="3">
         <v>37903</v>
       </c>
       <c r="B101">
@@ -1924,7 +1926,7 @@
       </c>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="4">
+      <c r="A102" s="3">
         <v>37904</v>
       </c>
       <c r="B102">
@@ -1938,7 +1940,7 @@
       </c>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="4">
+      <c r="A103" s="3">
         <v>37905</v>
       </c>
       <c r="B103">
@@ -1952,7 +1954,7 @@
       </c>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="4">
+      <c r="A104" s="3">
         <v>37906</v>
       </c>
       <c r="B104">
@@ -1966,7 +1968,7 @@
       </c>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="4">
+      <c r="A105" s="3">
         <v>37907</v>
       </c>
       <c r="B105">
@@ -1980,7 +1982,7 @@
       </c>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="4">
+      <c r="A106" s="3">
         <v>37908</v>
       </c>
       <c r="B106">
@@ -1994,7 +1996,7 @@
       </c>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="4">
+      <c r="A107" s="3">
         <v>37909</v>
       </c>
       <c r="B107">
@@ -2008,7 +2010,7 @@
       </c>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="4">
+      <c r="A108" s="3">
         <v>37910</v>
       </c>
       <c r="B108">
@@ -2022,7 +2024,7 @@
       </c>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="4">
+      <c r="A109" s="3">
         <v>37911</v>
       </c>
       <c r="B109">
@@ -2036,7 +2038,7 @@
       </c>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" s="4">
+      <c r="A110" s="3">
         <v>37912</v>
       </c>
       <c r="B110">
@@ -2050,7 +2052,7 @@
       </c>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" s="4">
+      <c r="A111" s="3">
         <v>37913</v>
       </c>
       <c r="B111">
@@ -2064,7 +2066,7 @@
       </c>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" s="4">
+      <c r="A112" s="3">
         <v>37914</v>
       </c>
       <c r="B112">
@@ -2078,7 +2080,7 @@
       </c>
     </row>
     <row r="113" spans="1:4">
-      <c r="A113" s="4">
+      <c r="A113" s="3">
         <v>37915</v>
       </c>
       <c r="B113">
@@ -2092,7 +2094,7 @@
       </c>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" s="4">
+      <c r="A114" s="3">
         <v>37916</v>
       </c>
       <c r="B114">
@@ -2106,7 +2108,7 @@
       </c>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" s="4">
+      <c r="A115" s="3">
         <v>37917</v>
       </c>
       <c r="B115">
@@ -2120,7 +2122,7 @@
       </c>
     </row>
     <row r="116" spans="1:4">
-      <c r="A116" s="4">
+      <c r="A116" s="3">
         <v>37918</v>
       </c>
       <c r="B116">
@@ -2134,7 +2136,7 @@
       </c>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" s="4">
+      <c r="A117" s="3">
         <v>37919</v>
       </c>
       <c r="B117">
@@ -2148,7 +2150,7 @@
       </c>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" s="4">
+      <c r="A118" s="3">
         <v>37920</v>
       </c>
       <c r="B118">
@@ -2162,7 +2164,7 @@
       </c>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" s="4">
+      <c r="A119" s="3">
         <v>37921</v>
       </c>
       <c r="B119">
@@ -2176,7 +2178,7 @@
       </c>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" s="4">
+      <c r="A120" s="3">
         <v>37922</v>
       </c>
       <c r="B120">
@@ -2190,7 +2192,7 @@
       </c>
     </row>
     <row r="121" spans="1:4">
-      <c r="A121" s="4">
+      <c r="A121" s="3">
         <v>37923</v>
       </c>
       <c r="B121">
@@ -2204,7 +2206,7 @@
       </c>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" s="4">
+      <c r="A122" s="3">
         <v>37924</v>
       </c>
       <c r="B122">
@@ -2218,7 +2220,7 @@
       </c>
     </row>
     <row r="123" spans="1:4">
-      <c r="A123" s="4">
+      <c r="A123" s="3">
         <v>37925</v>
       </c>
       <c r="B123">
@@ -2232,7 +2234,7 @@
       </c>
     </row>
     <row r="124" spans="1:4">
-      <c r="A124" s="4">
+      <c r="A124" s="3">
         <v>37926</v>
       </c>
       <c r="B124">
@@ -2246,7 +2248,7 @@
       </c>
     </row>
     <row r="125" spans="1:4">
-      <c r="A125" s="4">
+      <c r="A125" s="3">
         <v>37927</v>
       </c>
       <c r="B125">
@@ -2260,7 +2262,7 @@
       </c>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" s="4">
+      <c r="A126" s="3">
         <v>37928</v>
       </c>
       <c r="B126">
@@ -2274,7 +2276,7 @@
       </c>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" s="4">
+      <c r="A127" s="3">
         <v>37929</v>
       </c>
       <c r="B127">
@@ -2288,7 +2290,7 @@
       </c>
     </row>
     <row r="128" spans="1:4">
-      <c r="A128" s="4">
+      <c r="A128" s="3">
         <v>37930</v>
       </c>
       <c r="B128">
@@ -2302,7 +2304,7 @@
       </c>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" s="4">
+      <c r="A129" s="3">
         <v>37931</v>
       </c>
       <c r="B129">
@@ -2316,7 +2318,7 @@
       </c>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="4">
+      <c r="A130" s="3">
         <v>37932</v>
       </c>
       <c r="B130">
@@ -2330,7 +2332,7 @@
       </c>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="4">
+      <c r="A131" s="3">
         <v>37933</v>
       </c>
       <c r="B131">
@@ -2344,7 +2346,7 @@
       </c>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" s="4">
+      <c r="A132" s="3">
         <v>37934</v>
       </c>
       <c r="B132">
@@ -2358,7 +2360,7 @@
       </c>
     </row>
     <row r="133" spans="1:4">
-      <c r="A133" s="4">
+      <c r="A133" s="3">
         <v>37935</v>
       </c>
       <c r="B133">
@@ -2372,7 +2374,7 @@
       </c>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" s="4">
+      <c r="A134" s="3">
         <v>37936</v>
       </c>
       <c r="B134">
@@ -2386,7 +2388,7 @@
       </c>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" s="4">
+      <c r="A135" s="3">
         <v>37937</v>
       </c>
       <c r="B135">
@@ -2400,7 +2402,7 @@
       </c>
     </row>
     <row r="136" spans="1:4">
-      <c r="A136" s="4">
+      <c r="A136" s="3">
         <v>37938</v>
       </c>
       <c r="B136">
@@ -2414,7 +2416,7 @@
       </c>
     </row>
     <row r="137" spans="1:4">
-      <c r="A137" s="4">
+      <c r="A137" s="3">
         <v>37939</v>
       </c>
       <c r="B137">
@@ -2428,7 +2430,7 @@
       </c>
     </row>
     <row r="138" spans="1:4">
-      <c r="A138" s="4">
+      <c r="A138" s="3">
         <v>37940</v>
       </c>
       <c r="B138">
@@ -2442,7 +2444,7 @@
       </c>
     </row>
     <row r="139" spans="1:4">
-      <c r="A139" s="4">
+      <c r="A139" s="3">
         <v>37941</v>
       </c>
       <c r="B139">
@@ -2456,7 +2458,7 @@
       </c>
     </row>
     <row r="140" spans="1:4">
-      <c r="A140" s="4">
+      <c r="A140" s="3">
         <v>37942</v>
       </c>
       <c r="B140">
@@ -2470,7 +2472,7 @@
       </c>
     </row>
     <row r="141" spans="1:4">
-      <c r="A141" s="4">
+      <c r="A141" s="3">
         <v>37943</v>
       </c>
       <c r="B141">
@@ -2484,7 +2486,7 @@
       </c>
     </row>
     <row r="142" spans="1:4">
-      <c r="A142" s="4">
+      <c r="A142" s="3">
         <v>37944</v>
       </c>
       <c r="B142">
@@ -2498,7 +2500,7 @@
       </c>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="4">
+      <c r="A143" s="3">
         <v>37945</v>
       </c>
       <c r="B143">
@@ -2512,7 +2514,7 @@
       </c>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" s="4">
+      <c r="A144" s="3">
         <v>37946</v>
       </c>
       <c r="B144">
@@ -2526,7 +2528,7 @@
       </c>
     </row>
     <row r="145" spans="1:4">
-      <c r="A145" s="4">
+      <c r="A145" s="3">
         <v>37947</v>
       </c>
       <c r="B145">
@@ -2540,7 +2542,7 @@
       </c>
     </row>
     <row r="146" spans="1:4">
-      <c r="A146" s="4">
+      <c r="A146" s="3">
         <v>37948</v>
       </c>
       <c r="B146">
@@ -2554,7 +2556,7 @@
       </c>
     </row>
     <row r="147" spans="1:4">
-      <c r="A147" s="4">
+      <c r="A147" s="3">
         <v>37949</v>
       </c>
       <c r="B147">
@@ -2568,7 +2570,7 @@
       </c>
     </row>
     <row r="148" spans="1:4">
-      <c r="A148" s="4">
+      <c r="A148" s="3">
         <v>37950</v>
       </c>
       <c r="B148">
@@ -2582,7 +2584,7 @@
       </c>
     </row>
     <row r="149" spans="1:4">
-      <c r="A149" s="4">
+      <c r="A149" s="3">
         <v>37951</v>
       </c>
       <c r="B149">
@@ -2596,7 +2598,7 @@
       </c>
     </row>
     <row r="150" spans="1:4">
-      <c r="A150" s="4">
+      <c r="A150" s="3">
         <v>37952</v>
       </c>
       <c r="B150">
@@ -2610,7 +2612,7 @@
       </c>
     </row>
     <row r="151" spans="1:4">
-      <c r="A151" s="4">
+      <c r="A151" s="3">
         <v>37953</v>
       </c>
       <c r="B151">
@@ -2624,7 +2626,7 @@
       </c>
     </row>
     <row r="152" spans="1:4">
-      <c r="A152" s="4">
+      <c r="A152" s="3">
         <v>37954</v>
       </c>
       <c r="B152">
@@ -2638,7 +2640,7 @@
       </c>
     </row>
     <row r="153" spans="1:4">
-      <c r="A153" s="4">
+      <c r="A153" s="3">
         <v>37955</v>
       </c>
       <c r="B153">
@@ -2652,7 +2654,7 @@
       </c>
     </row>
     <row r="154" spans="1:4">
-      <c r="A154" s="4">
+      <c r="A154" s="3">
         <v>37956</v>
       </c>
       <c r="B154">
@@ -2666,7 +2668,7 @@
       </c>
     </row>
     <row r="155" spans="1:4">
-      <c r="A155" s="4">
+      <c r="A155" s="3">
         <v>37957</v>
       </c>
       <c r="B155">
@@ -2680,7 +2682,7 @@
       </c>
     </row>
     <row r="156" spans="1:4">
-      <c r="A156" s="4">
+      <c r="A156" s="3">
         <v>37958</v>
       </c>
       <c r="B156">
@@ -2694,7 +2696,7 @@
       </c>
     </row>
     <row r="157" spans="1:4">
-      <c r="A157" s="4">
+      <c r="A157" s="3">
         <v>37959</v>
       </c>
       <c r="B157">
@@ -2708,7 +2710,7 @@
       </c>
     </row>
     <row r="158" spans="1:4">
-      <c r="A158" s="4">
+      <c r="A158" s="3">
         <v>37960</v>
       </c>
       <c r="B158">
@@ -2722,7 +2724,7 @@
       </c>
     </row>
     <row r="159" spans="1:4">
-      <c r="A159" s="4">
+      <c r="A159" s="3">
         <v>37961</v>
       </c>
       <c r="B159">
@@ -2736,7 +2738,7 @@
       </c>
     </row>
     <row r="160" spans="1:4">
-      <c r="A160" s="4">
+      <c r="A160" s="3">
         <v>37962</v>
       </c>
       <c r="B160">
@@ -2750,7 +2752,7 @@
       </c>
     </row>
     <row r="161" spans="1:4">
-      <c r="A161" s="4">
+      <c r="A161" s="3">
         <v>37963</v>
       </c>
       <c r="B161">
@@ -2764,7 +2766,7 @@
       </c>
     </row>
     <row r="162" spans="1:4">
-      <c r="A162" s="4">
+      <c r="A162" s="3">
         <v>37964</v>
       </c>
       <c r="B162">
@@ -2778,7 +2780,7 @@
       </c>
     </row>
     <row r="163" spans="1:4">
-      <c r="A163" s="4">
+      <c r="A163" s="3">
         <v>37965</v>
       </c>
       <c r="B163">
@@ -2792,7 +2794,7 @@
       </c>
     </row>
     <row r="164" spans="1:4">
-      <c r="A164" s="4">
+      <c r="A164" s="3">
         <v>37966</v>
       </c>
       <c r="B164">
@@ -2806,7 +2808,7 @@
       </c>
     </row>
     <row r="165" spans="1:4">
-      <c r="A165" s="4">
+      <c r="A165" s="3">
         <v>37967</v>
       </c>
       <c r="B165">
@@ -2820,7 +2822,7 @@
       </c>
     </row>
     <row r="166" spans="1:4">
-      <c r="A166" s="4">
+      <c r="A166" s="3">
         <v>37968</v>
       </c>
       <c r="B166">
@@ -2834,7 +2836,7 @@
       </c>
     </row>
     <row r="167" spans="1:4">
-      <c r="A167" s="4">
+      <c r="A167" s="3">
         <v>37969</v>
       </c>
       <c r="B167">
@@ -2848,7 +2850,7 @@
       </c>
     </row>
     <row r="168" spans="1:4">
-      <c r="A168" s="4">
+      <c r="A168" s="3">
         <v>37970</v>
       </c>
       <c r="B168">
@@ -2862,7 +2864,7 @@
       </c>
     </row>
     <row r="169" spans="1:4">
-      <c r="A169" s="4">
+      <c r="A169" s="3">
         <v>37971</v>
       </c>
       <c r="B169">
@@ -2876,7 +2878,7 @@
       </c>
     </row>
     <row r="170" spans="1:4">
-      <c r="A170" s="4">
+      <c r="A170" s="3">
         <v>37972</v>
       </c>
       <c r="B170">
@@ -2890,7 +2892,7 @@
       </c>
     </row>
     <row r="171" spans="1:4">
-      <c r="A171" s="4">
+      <c r="A171" s="3">
         <v>37973</v>
       </c>
       <c r="B171">
@@ -2904,7 +2906,7 @@
       </c>
     </row>
     <row r="172" spans="1:4">
-      <c r="A172" s="4">
+      <c r="A172" s="3">
         <v>37974</v>
       </c>
       <c r="B172">
@@ -2918,7 +2920,7 @@
       </c>
     </row>
     <row r="173" spans="1:4">
-      <c r="A173" s="4">
+      <c r="A173" s="3">
         <v>37975</v>
       </c>
       <c r="B173">
@@ -2932,7 +2934,7 @@
       </c>
     </row>
     <row r="174" spans="1:4">
-      <c r="A174" s="4">
+      <c r="A174" s="3">
         <v>37976</v>
       </c>
       <c r="B174">
@@ -2946,7 +2948,7 @@
       </c>
     </row>
     <row r="175" spans="1:4">
-      <c r="A175" s="4">
+      <c r="A175" s="3">
         <v>37977</v>
       </c>
       <c r="B175">
@@ -2960,7 +2962,7 @@
       </c>
     </row>
     <row r="176" spans="1:4">
-      <c r="A176" s="4">
+      <c r="A176" s="3">
         <v>37978</v>
       </c>
       <c r="B176">
@@ -2974,7 +2976,7 @@
       </c>
     </row>
     <row r="177" spans="1:4">
-      <c r="A177" s="4">
+      <c r="A177" s="3">
         <v>37979</v>
       </c>
       <c r="B177">
@@ -2988,7 +2990,7 @@
       </c>
     </row>
     <row r="178" spans="1:4">
-      <c r="A178" s="4">
+      <c r="A178" s="3">
         <v>37980</v>
       </c>
       <c r="B178">
@@ -3002,7 +3004,7 @@
       </c>
     </row>
     <row r="179" spans="1:4">
-      <c r="A179" s="4">
+      <c r="A179" s="3">
         <v>37981</v>
       </c>
       <c r="B179">
@@ -3016,7 +3018,7 @@
       </c>
     </row>
     <row r="180" spans="1:4">
-      <c r="A180" s="4">
+      <c r="A180" s="3">
         <v>37982</v>
       </c>
       <c r="B180">
@@ -3030,7 +3032,7 @@
       </c>
     </row>
     <row r="181" spans="1:4">
-      <c r="A181" s="4">
+      <c r="A181" s="3">
         <v>37983</v>
       </c>
       <c r="B181">
@@ -3044,7 +3046,7 @@
       </c>
     </row>
     <row r="182" spans="1:4">
-      <c r="A182" s="4">
+      <c r="A182" s="3">
         <v>37984</v>
       </c>
       <c r="B182">
@@ -3058,7 +3060,7 @@
       </c>
     </row>
     <row r="183" spans="1:4">
-      <c r="A183" s="4">
+      <c r="A183" s="3">
         <v>37985</v>
       </c>
       <c r="B183">
@@ -3072,7 +3074,7 @@
       </c>
     </row>
     <row r="184" spans="1:4">
-      <c r="A184" s="4">
+      <c r="A184" s="3">
         <v>37986</v>
       </c>
       <c r="B184">
@@ -3086,7 +3088,7 @@
       </c>
     </row>
     <row r="185" spans="1:4">
-      <c r="A185" s="4">
+      <c r="A185" s="3">
         <v>37987</v>
       </c>
       <c r="B185">
@@ -3100,7 +3102,7 @@
       </c>
     </row>
     <row r="186" spans="1:4">
-      <c r="A186" s="4">
+      <c r="A186" s="3">
         <v>37988</v>
       </c>
       <c r="B186">
@@ -3114,7 +3116,7 @@
       </c>
     </row>
     <row r="187" spans="1:4">
-      <c r="A187" s="4">
+      <c r="A187" s="3">
         <v>37989</v>
       </c>
       <c r="B187">
@@ -3128,7 +3130,7 @@
       </c>
     </row>
     <row r="188" spans="1:4">
-      <c r="A188" s="4">
+      <c r="A188" s="3">
         <v>37990</v>
       </c>
       <c r="B188">
@@ -3142,7 +3144,7 @@
       </c>
     </row>
     <row r="189" spans="1:4">
-      <c r="A189" s="4">
+      <c r="A189" s="3">
         <v>37991</v>
       </c>
       <c r="B189">
@@ -3156,7 +3158,7 @@
       </c>
     </row>
     <row r="190" spans="1:4">
-      <c r="A190" s="4">
+      <c r="A190" s="3">
         <v>37992</v>
       </c>
       <c r="B190">
@@ -3170,7 +3172,7 @@
       </c>
     </row>
     <row r="191" spans="1:4">
-      <c r="A191" s="4">
+      <c r="A191" s="3">
         <v>37993</v>
       </c>
       <c r="B191">
@@ -3184,7 +3186,7 @@
       </c>
     </row>
     <row r="192" spans="1:4">
-      <c r="A192" s="4">
+      <c r="A192" s="3">
         <v>37994</v>
       </c>
       <c r="B192">
@@ -3198,7 +3200,7 @@
       </c>
     </row>
     <row r="193" spans="1:4">
-      <c r="A193" s="4">
+      <c r="A193" s="3">
         <v>37995</v>
       </c>
       <c r="B193">
@@ -3212,7 +3214,7 @@
       </c>
     </row>
     <row r="194" spans="1:4">
-      <c r="A194" s="4">
+      <c r="A194" s="3">
         <v>37996</v>
       </c>
       <c r="B194">
@@ -3226,7 +3228,7 @@
       </c>
     </row>
     <row r="195" spans="1:4">
-      <c r="A195" s="4">
+      <c r="A195" s="3">
         <v>37997</v>
       </c>
       <c r="B195">
@@ -3240,7 +3242,7 @@
       </c>
     </row>
     <row r="196" spans="1:4">
-      <c r="A196" s="4">
+      <c r="A196" s="3">
         <v>37998</v>
       </c>
       <c r="B196">
@@ -3254,7 +3256,7 @@
       </c>
     </row>
     <row r="197" spans="1:4">
-      <c r="A197" s="4">
+      <c r="A197" s="3">
         <v>37999</v>
       </c>
       <c r="B197">
@@ -3268,7 +3270,7 @@
       </c>
     </row>
     <row r="198" spans="1:4">
-      <c r="A198" s="4">
+      <c r="A198" s="3">
         <v>38000</v>
       </c>
       <c r="B198">
@@ -3282,7 +3284,7 @@
       </c>
     </row>
     <row r="199" spans="1:4">
-      <c r="A199" s="4">
+      <c r="A199" s="3">
         <v>38001</v>
       </c>
       <c r="B199">
@@ -3296,7 +3298,7 @@
       </c>
     </row>
     <row r="200" spans="1:4">
-      <c r="A200" s="4">
+      <c r="A200" s="3">
         <v>38002</v>
       </c>
       <c r="B200">
@@ -3310,7 +3312,7 @@
       </c>
     </row>
     <row r="201" spans="1:4">
-      <c r="A201" s="4">
+      <c r="A201" s="3">
         <v>38003</v>
       </c>
       <c r="B201">
@@ -3324,7 +3326,7 @@
       </c>
     </row>
     <row r="202" spans="1:4">
-      <c r="A202" s="4">
+      <c r="A202" s="3">
         <v>38004</v>
       </c>
       <c r="B202">
@@ -3338,7 +3340,7 @@
       </c>
     </row>
     <row r="203" spans="1:4">
-      <c r="A203" s="4">
+      <c r="A203" s="3">
         <v>38005</v>
       </c>
       <c r="B203">
@@ -3352,7 +3354,7 @@
       </c>
     </row>
     <row r="204" spans="1:4">
-      <c r="A204" s="4">
+      <c r="A204" s="3">
         <v>38006</v>
       </c>
       <c r="B204">
@@ -3366,7 +3368,7 @@
       </c>
     </row>
     <row r="205" spans="1:4">
-      <c r="A205" s="4">
+      <c r="A205" s="3">
         <v>38007</v>
       </c>
       <c r="B205">
@@ -3380,7 +3382,7 @@
       </c>
     </row>
     <row r="206" spans="1:4">
-      <c r="A206" s="4">
+      <c r="A206" s="3">
         <v>38008</v>
       </c>
       <c r="B206">
@@ -3394,7 +3396,7 @@
       </c>
     </row>
     <row r="207" spans="1:4">
-      <c r="A207" s="4">
+      <c r="A207" s="3">
         <v>38009</v>
       </c>
       <c r="B207">
@@ -3408,7 +3410,7 @@
       </c>
     </row>
     <row r="208" spans="1:4">
-      <c r="A208" s="4">
+      <c r="A208" s="3">
         <v>38010</v>
       </c>
       <c r="B208">
@@ -3422,7 +3424,7 @@
       </c>
     </row>
     <row r="209" spans="1:4">
-      <c r="A209" s="4">
+      <c r="A209" s="3">
         <v>38011</v>
       </c>
       <c r="B209">
@@ -3436,7 +3438,7 @@
       </c>
     </row>
     <row r="210" spans="1:4">
-      <c r="A210" s="4">
+      <c r="A210" s="3">
         <v>38012</v>
       </c>
       <c r="B210">
@@ -3450,7 +3452,7 @@
       </c>
     </row>
     <row r="211" spans="1:4">
-      <c r="A211" s="4">
+      <c r="A211" s="3">
         <v>38013</v>
       </c>
       <c r="B211">
@@ -3464,7 +3466,7 @@
       </c>
     </row>
     <row r="212" spans="1:4">
-      <c r="A212" s="4">
+      <c r="A212" s="3">
         <v>38014</v>
       </c>
       <c r="B212">
@@ -3478,7 +3480,7 @@
       </c>
     </row>
     <row r="213" spans="1:4">
-      <c r="A213" s="4">
+      <c r="A213" s="3">
         <v>38015</v>
       </c>
       <c r="B213">
@@ -3492,7 +3494,7 @@
       </c>
     </row>
     <row r="214" spans="1:4">
-      <c r="A214" s="4">
+      <c r="A214" s="3">
         <v>38016</v>
       </c>
       <c r="B214">
@@ -3506,7 +3508,7 @@
       </c>
     </row>
     <row r="215" spans="1:4">
-      <c r="A215" s="4">
+      <c r="A215" s="3">
         <v>38017</v>
       </c>
       <c r="B215">
@@ -3520,7 +3522,7 @@
       </c>
     </row>
     <row r="216" spans="1:4">
-      <c r="A216" s="4">
+      <c r="A216" s="3">
         <v>38018</v>
       </c>
       <c r="B216">
@@ -3534,7 +3536,7 @@
       </c>
     </row>
     <row r="217" spans="1:4">
-      <c r="A217" s="4">
+      <c r="A217" s="3">
         <v>38019</v>
       </c>
       <c r="B217">
@@ -3548,7 +3550,7 @@
       </c>
     </row>
     <row r="218" spans="1:4">
-      <c r="A218" s="4">
+      <c r="A218" s="3">
         <v>38020</v>
       </c>
       <c r="B218">
@@ -3562,7 +3564,7 @@
       </c>
     </row>
     <row r="219" spans="1:4">
-      <c r="A219" s="4">
+      <c r="A219" s="3">
         <v>38021</v>
       </c>
       <c r="B219">
@@ -3576,7 +3578,7 @@
       </c>
     </row>
     <row r="220" spans="1:4">
-      <c r="A220" s="4">
+      <c r="A220" s="3">
         <v>38022</v>
       </c>
       <c r="B220">
@@ -3590,7 +3592,7 @@
       </c>
     </row>
     <row r="221" spans="1:4">
-      <c r="A221" s="4">
+      <c r="A221" s="3">
         <v>38023</v>
       </c>
       <c r="B221">
@@ -3604,7 +3606,7 @@
       </c>
     </row>
     <row r="222" spans="1:4">
-      <c r="A222" s="4">
+      <c r="A222" s="3">
         <v>38024</v>
       </c>
       <c r="B222">
@@ -3618,7 +3620,7 @@
       </c>
     </row>
     <row r="223" spans="1:4">
-      <c r="A223" s="4">
+      <c r="A223" s="3">
         <v>38025</v>
       </c>
       <c r="B223">
@@ -3632,7 +3634,7 @@
       </c>
     </row>
     <row r="224" spans="1:4">
-      <c r="A224" s="4">
+      <c r="A224" s="3">
         <v>38026</v>
       </c>
       <c r="B224">
@@ -3646,7 +3648,7 @@
       </c>
     </row>
     <row r="225" spans="1:4">
-      <c r="A225" s="4">
+      <c r="A225" s="3">
         <v>38027</v>
       </c>
       <c r="B225">
@@ -3660,7 +3662,7 @@
       </c>
     </row>
     <row r="226" spans="1:4">
-      <c r="A226" s="4">
+      <c r="A226" s="3">
         <v>38028</v>
       </c>
       <c r="B226">
@@ -3674,7 +3676,7 @@
       </c>
     </row>
     <row r="227" spans="1:4">
-      <c r="A227" s="4">
+      <c r="A227" s="3">
         <v>38029</v>
       </c>
       <c r="B227">
@@ -3688,7 +3690,7 @@
       </c>
     </row>
     <row r="228" spans="1:4">
-      <c r="A228" s="4">
+      <c r="A228" s="3">
         <v>38030</v>
       </c>
       <c r="B228">
@@ -3702,7 +3704,7 @@
       </c>
     </row>
     <row r="229" spans="1:4">
-      <c r="A229" s="4">
+      <c r="A229" s="3">
         <v>38031</v>
       </c>
       <c r="B229">
@@ -3716,7 +3718,7 @@
       </c>
     </row>
     <row r="230" spans="1:4">
-      <c r="A230" s="4">
+      <c r="A230" s="3">
         <v>38032</v>
       </c>
       <c r="B230">
@@ -3730,7 +3732,7 @@
       </c>
     </row>
     <row r="231" spans="1:4">
-      <c r="A231" s="4">
+      <c r="A231" s="3">
         <v>38033</v>
       </c>
       <c r="B231">
@@ -3744,7 +3746,7 @@
       </c>
     </row>
     <row r="232" spans="1:4">
-      <c r="A232" s="4">
+      <c r="A232" s="3">
         <v>38034</v>
       </c>
       <c r="B232">
@@ -3758,7 +3760,7 @@
       </c>
     </row>
     <row r="233" spans="1:4">
-      <c r="A233" s="4">
+      <c r="A233" s="3">
         <v>38035</v>
       </c>
       <c r="B233">
@@ -3772,7 +3774,7 @@
       </c>
     </row>
     <row r="234" spans="1:4">
-      <c r="A234" s="4">
+      <c r="A234" s="3">
         <v>38036</v>
       </c>
       <c r="B234">
@@ -3786,7 +3788,7 @@
       </c>
     </row>
     <row r="235" spans="1:4">
-      <c r="A235" s="4">
+      <c r="A235" s="3">
         <v>38037</v>
       </c>
       <c r="B235">
@@ -3800,7 +3802,7 @@
       </c>
     </row>
     <row r="236" spans="1:4">
-      <c r="A236" s="4">
+      <c r="A236" s="3">
         <v>38038</v>
       </c>
       <c r="B236">
@@ -3814,7 +3816,7 @@
       </c>
     </row>
     <row r="237" spans="1:4">
-      <c r="A237" s="4">
+      <c r="A237" s="3">
         <v>38039</v>
       </c>
       <c r="B237">
@@ -3828,7 +3830,7 @@
       </c>
     </row>
     <row r="238" spans="1:4">
-      <c r="A238" s="4">
+      <c r="A238" s="3">
         <v>38040</v>
       </c>
       <c r="B238">
@@ -3842,7 +3844,7 @@
       </c>
     </row>
     <row r="239" spans="1:4">
-      <c r="A239" s="4">
+      <c r="A239" s="3">
         <v>38041</v>
       </c>
       <c r="B239">
@@ -3856,7 +3858,7 @@
       </c>
     </row>
     <row r="240" spans="1:4">
-      <c r="A240" s="4">
+      <c r="A240" s="3">
         <v>38042</v>
       </c>
       <c r="B240">
@@ -3870,7 +3872,7 @@
       </c>
     </row>
     <row r="241" spans="1:4">
-      <c r="A241" s="4">
+      <c r="A241" s="3">
         <v>38043</v>
       </c>
       <c r="B241">
@@ -3884,7 +3886,7 @@
       </c>
     </row>
     <row r="242" spans="1:4">
-      <c r="A242" s="4">
+      <c r="A242" s="3">
         <v>38044</v>
       </c>
       <c r="B242">
@@ -3898,7 +3900,7 @@
       </c>
     </row>
     <row r="243" spans="1:4">
-      <c r="A243" s="4">
+      <c r="A243" s="3">
         <v>38045</v>
       </c>
       <c r="B243">
@@ -3912,7 +3914,7 @@
       </c>
     </row>
     <row r="244" spans="1:4">
-      <c r="A244" s="4">
+      <c r="A244" s="3">
         <v>38046</v>
       </c>
       <c r="B244">
@@ -3926,7 +3928,7 @@
       </c>
     </row>
     <row r="245" spans="1:4">
-      <c r="A245" s="4">
+      <c r="A245" s="3">
         <v>38047</v>
       </c>
       <c r="B245">
@@ -3940,7 +3942,7 @@
       </c>
     </row>
     <row r="246" spans="1:4">
-      <c r="A246" s="4">
+      <c r="A246" s="3">
         <v>38048</v>
       </c>
       <c r="B246">
@@ -3954,1571 +3956,1571 @@
       </c>
     </row>
     <row r="247" spans="1:4">
-      <c r="A247" s="4">
+      <c r="A247" s="3">
         <v>38049</v>
       </c>
       <c r="B247">
-        <v>111049.37</v>
+        <v>111049.22</v>
       </c>
       <c r="C247" s="1">
-        <v>0.002793117504180653</v>
+        <v>0.002791762980803858</v>
       </c>
       <c r="D247" s="1">
-        <v>0.1104936999999997</v>
+        <v>0.1104921999999997</v>
       </c>
     </row>
     <row r="248" spans="1:4">
-      <c r="A248" s="4">
+      <c r="A248" s="3">
         <v>38050</v>
       </c>
       <c r="B248">
-        <v>111276.92</v>
+        <v>111276.77</v>
       </c>
       <c r="C248" s="1">
-        <v>0.00204908861707187</v>
+        <v>0.002049091384883184</v>
       </c>
       <c r="D248" s="1">
-        <v>0.1127691999999998</v>
+        <v>0.1127676999999996</v>
       </c>
     </row>
     <row r="249" spans="1:4">
-      <c r="A249" s="4">
+      <c r="A249" s="3">
         <v>38051</v>
       </c>
       <c r="B249">
-        <v>111572.25</v>
+        <v>111572.1</v>
       </c>
       <c r="C249" s="1">
-        <v>0.002654009474741148</v>
+        <v>0.002654013052319826</v>
       </c>
       <c r="D249" s="1">
-        <v>0.1157225</v>
+        <v>0.1157209999999995</v>
       </c>
     </row>
     <row r="250" spans="1:4">
-      <c r="A250" s="4">
+      <c r="A250" s="3">
         <v>38052</v>
       </c>
       <c r="B250">
-        <v>111572.25</v>
+        <v>111572.1</v>
       </c>
       <c r="C250" s="1">
         <v>0</v>
       </c>
       <c r="D250" s="1">
-        <v>0.1157225</v>
+        <v>0.1157209999999995</v>
       </c>
     </row>
     <row r="251" spans="1:4">
-      <c r="A251" s="4">
+      <c r="A251" s="3">
         <v>38053</v>
       </c>
       <c r="B251">
-        <v>111572.25</v>
+        <v>111572.1</v>
       </c>
       <c r="C251" s="1">
         <v>0</v>
       </c>
       <c r="D251" s="1">
-        <v>0.1157225</v>
+        <v>0.1157209999999995</v>
       </c>
     </row>
     <row r="252" spans="1:4">
-      <c r="A252" s="4">
+      <c r="A252" s="3">
         <v>38054</v>
       </c>
       <c r="B252">
-        <v>111172.15</v>
+        <v>111172</v>
       </c>
       <c r="C252" s="1">
-        <v>-0.003586017132396369</v>
+        <v>-0.003586021953517093</v>
       </c>
       <c r="D252" s="1">
-        <v>0.1117214999999998</v>
+        <v>0.1117199999999994</v>
       </c>
     </row>
     <row r="253" spans="1:4">
-      <c r="A253" s="4">
+      <c r="A253" s="3">
         <v>38055</v>
       </c>
       <c r="B253">
-        <v>110721.5</v>
+        <v>110721.35</v>
       </c>
       <c r="C253" s="1">
-        <v>-0.004053623142126983</v>
+        <v>-0.004053628611520921</v>
       </c>
       <c r="D253" s="1">
-        <v>0.1072149999999996</v>
+        <v>0.1072134999999994</v>
       </c>
     </row>
     <row r="254" spans="1:4">
-      <c r="A254" s="4">
+      <c r="A254" s="3">
         <v>38056</v>
       </c>
       <c r="B254">
-        <v>109558.91</v>
+        <v>109558.76</v>
       </c>
       <c r="C254" s="1">
-        <v>-0.01050012870129102</v>
+        <v>-0.01050014292636425</v>
       </c>
       <c r="D254" s="1">
-        <v>0.09558909999999976</v>
+        <v>0.09558759999999933</v>
       </c>
     </row>
     <row r="255" spans="1:4">
-      <c r="A255" s="4">
+      <c r="A255" s="3">
         <v>38057</v>
       </c>
       <c r="B255">
-        <v>107956.52</v>
+        <v>107956.37</v>
       </c>
       <c r="C255" s="1">
-        <v>-0.01462583006712992</v>
+        <v>-0.01462585009176798</v>
       </c>
       <c r="D255" s="1">
-        <v>0.0795652</v>
+        <v>0.07956369999999957</v>
       </c>
     </row>
     <row r="256" spans="1:4">
-      <c r="A256" s="4">
+      <c r="A256" s="3">
         <v>38058</v>
       </c>
       <c r="B256">
-        <v>108683.9</v>
+        <v>108683.75</v>
       </c>
       <c r="C256" s="1">
-        <v>0.00673771255316491</v>
+        <v>0.006737721914880979</v>
       </c>
       <c r="D256" s="1">
-        <v>0.08683899999999989</v>
+        <v>0.08683749999999946</v>
       </c>
     </row>
     <row r="257" spans="1:4">
-      <c r="A257" s="4">
+      <c r="A257" s="3">
         <v>38059</v>
       </c>
       <c r="B257">
-        <v>108683.9</v>
+        <v>108683.75</v>
       </c>
       <c r="C257" s="1">
         <v>0</v>
       </c>
       <c r="D257" s="1">
-        <v>0.08683899999999989</v>
+        <v>0.08683749999999946</v>
       </c>
     </row>
     <row r="258" spans="1:4">
-      <c r="A258" s="4">
+      <c r="A258" s="3">
         <v>38060</v>
       </c>
       <c r="B258">
-        <v>108683.9</v>
+        <v>108683.75</v>
       </c>
       <c r="C258" s="1">
         <v>0</v>
       </c>
       <c r="D258" s="1">
-        <v>0.08683899999999989</v>
+        <v>0.08683749999999946</v>
       </c>
     </row>
     <row r="259" spans="1:4">
-      <c r="A259" s="4">
+      <c r="A259" s="3">
         <v>38061</v>
       </c>
       <c r="B259">
-        <v>107632.42</v>
+        <v>107632.27</v>
       </c>
       <c r="C259" s="1">
-        <v>-0.009674662024458214</v>
+        <v>-0.009674675376953878</v>
       </c>
       <c r="D259" s="1">
-        <v>0.07632419999999973</v>
+        <v>0.0763226999999993</v>
       </c>
     </row>
     <row r="260" spans="1:4">
-      <c r="A260" s="4">
+      <c r="A260" s="3">
         <v>38062</v>
       </c>
       <c r="B260">
-        <v>108072.71</v>
+        <v>108072.56</v>
       </c>
       <c r="C260" s="1">
-        <v>0.004090681971101295</v>
+        <v>0.004090687672015259</v>
       </c>
       <c r="D260" s="1">
-        <v>0.08072709999999983</v>
+        <v>0.0807255999999994</v>
       </c>
     </row>
     <row r="261" spans="1:4">
-      <c r="A261" s="4">
+      <c r="A261" s="3">
         <v>38063</v>
       </c>
       <c r="B261">
-        <v>109062.37</v>
+        <v>109062.22</v>
       </c>
       <c r="C261" s="1">
-        <v>0.009157353415121916</v>
+        <v>0.009157366125129185</v>
       </c>
       <c r="D261" s="1">
-        <v>0.09062369999999964</v>
+        <v>0.09062219999999921</v>
       </c>
     </row>
     <row r="262" spans="1:4">
-      <c r="A262" s="4">
+      <c r="A262" s="3">
         <v>38064</v>
       </c>
       <c r="B262">
-        <v>108923.23</v>
+        <v>108923.08</v>
       </c>
       <c r="C262" s="1">
-        <v>-0.001275783755661952</v>
+        <v>-0.001275785510326144</v>
       </c>
       <c r="D262" s="1">
-        <v>0.08923229999999971</v>
+        <v>0.08923079999999928</v>
       </c>
     </row>
     <row r="263" spans="1:4">
-      <c r="A263" s="4">
+      <c r="A263" s="3">
         <v>38065</v>
       </c>
       <c r="B263">
-        <v>108056.39</v>
+        <v>108056.24</v>
       </c>
       <c r="C263" s="1">
-        <v>-0.007958265651872298</v>
+        <v>-0.007958276611347959</v>
       </c>
       <c r="D263" s="1">
-        <v>0.0805638999999998</v>
+        <v>0.08056239999999937</v>
       </c>
     </row>
     <row r="264" spans="1:4">
-      <c r="A264" s="4">
+      <c r="A264" s="3">
         <v>38066</v>
       </c>
       <c r="B264">
-        <v>108056.39</v>
+        <v>108056.24</v>
       </c>
       <c r="C264" s="1">
         <v>0</v>
       </c>
       <c r="D264" s="1">
-        <v>0.0805638999999998</v>
+        <v>0.08056239999999937</v>
       </c>
     </row>
     <row r="265" spans="1:4">
-      <c r="A265" s="4">
+      <c r="A265" s="3">
         <v>38067</v>
       </c>
       <c r="B265">
-        <v>108056.39</v>
+        <v>108056.24</v>
       </c>
       <c r="C265" s="1">
         <v>0</v>
       </c>
       <c r="D265" s="1">
-        <v>0.0805638999999998</v>
+        <v>0.08056239999999937</v>
       </c>
     </row>
     <row r="266" spans="1:4">
-      <c r="A266" s="4">
+      <c r="A266" s="3">
         <v>38068</v>
       </c>
       <c r="B266">
-        <v>106923.63</v>
+        <v>106923.48</v>
       </c>
       <c r="C266" s="1">
-        <v>-0.01048304501010999</v>
+        <v>-0.01048305956231677</v>
       </c>
       <c r="D266" s="1">
-        <v>0.06923629999999981</v>
+        <v>0.06923479999999937</v>
       </c>
     </row>
     <row r="267" spans="1:4">
-      <c r="A267" s="4">
+      <c r="A267" s="3">
         <v>38069</v>
       </c>
       <c r="B267">
-        <v>106887.69</v>
+        <v>106887.54</v>
       </c>
       <c r="C267" s="1">
-        <v>-0.0003361277577276223</v>
+        <v>-0.0003361282292719814</v>
       </c>
       <c r="D267" s="1">
-        <v>0.0688768999999998</v>
+        <v>0.06887539999999936</v>
       </c>
     </row>
     <row r="268" spans="1:4">
-      <c r="A268" s="4">
+      <c r="A268" s="3">
         <v>38070</v>
       </c>
       <c r="B268">
-        <v>106652.88</v>
+        <v>106652.73</v>
       </c>
       <c r="C268" s="1">
-        <v>-0.002196791791459152</v>
+        <v>-0.002196794874313901</v>
       </c>
       <c r="D268" s="1">
-        <v>0.0665287999999995</v>
+        <v>0.06652729999999907</v>
       </c>
     </row>
     <row r="269" spans="1:4">
-      <c r="A269" s="4">
+      <c r="A269" s="3">
         <v>38071</v>
       </c>
       <c r="B269">
-        <v>107757.0100000001</v>
+        <v>107756.86</v>
       </c>
       <c r="C269" s="1">
-        <v>0.01035255681796898</v>
+        <v>0.01035257137815448</v>
       </c>
       <c r="D269" s="1">
-        <v>0.07757009999999975</v>
+        <v>0.07756859999999954</v>
       </c>
     </row>
     <row r="270" spans="1:4">
-      <c r="A270" s="4">
+      <c r="A270" s="3">
         <v>38072</v>
       </c>
       <c r="B270">
-        <v>107647.62</v>
+        <v>107647.47</v>
       </c>
       <c r="C270" s="1">
-        <v>-0.001015154373715577</v>
+        <v>-0.001015155786833533</v>
       </c>
       <c r="D270" s="1">
-        <v>0.07647619999999966</v>
+        <v>0.07647469999999945</v>
       </c>
     </row>
     <row r="271" spans="1:4">
-      <c r="A271" s="4">
+      <c r="A271" s="3">
         <v>38073</v>
       </c>
       <c r="B271">
-        <v>107647.62</v>
+        <v>107647.47</v>
       </c>
       <c r="C271" s="1">
         <v>0</v>
       </c>
       <c r="D271" s="1">
-        <v>0.07647619999999966</v>
+        <v>0.07647469999999945</v>
       </c>
     </row>
     <row r="272" spans="1:4">
-      <c r="A272" s="4">
+      <c r="A272" s="3">
         <v>38074</v>
       </c>
       <c r="B272">
-        <v>107647.62</v>
+        <v>107647.47</v>
       </c>
       <c r="C272" s="1">
         <v>0</v>
       </c>
       <c r="D272" s="1">
-        <v>0.07647619999999966</v>
+        <v>0.07647469999999945</v>
       </c>
     </row>
     <row r="273" spans="1:4">
-      <c r="A273" s="4">
+      <c r="A273" s="3">
         <v>38075</v>
       </c>
       <c r="B273">
-        <v>108825.82</v>
+        <v>108825.67</v>
       </c>
       <c r="C273" s="1">
-        <v>0.01094497026501839</v>
+        <v>0.01094498551614809</v>
       </c>
       <c r="D273" s="1">
-        <v>0.08825819999999962</v>
+        <v>0.08825669999999941</v>
       </c>
     </row>
     <row r="274" spans="1:4">
-      <c r="A274" s="4">
+      <c r="A274" s="3">
         <v>38076</v>
       </c>
       <c r="B274">
-        <v>109159.96</v>
+        <v>109159.81</v>
       </c>
       <c r="C274" s="1">
-        <v>0.00307041104767225</v>
+        <v>0.003070415279777361</v>
       </c>
       <c r="D274" s="1">
-        <v>0.09159959999999945</v>
+        <v>0.09159809999999946</v>
       </c>
     </row>
     <row r="275" spans="1:4">
-      <c r="A275" s="4">
+      <c r="A275" s="3">
         <v>38077</v>
       </c>
       <c r="B275">
-        <v>109212.28</v>
+        <v>109212.13</v>
       </c>
       <c r="C275" s="1">
-        <v>0.0004792966212154859</v>
+        <v>0.0004792972798322026</v>
       </c>
       <c r="D275" s="1">
-        <v>0.09212279999999962</v>
+        <v>0.09212129999999941</v>
       </c>
     </row>
     <row r="276" spans="1:4">
-      <c r="A276" s="4">
+      <c r="A276" s="3">
         <v>38078</v>
       </c>
       <c r="B276">
-        <v>109659.8</v>
+        <v>109659.65</v>
       </c>
       <c r="C276" s="1">
-        <v>0.004097707693676789</v>
+        <v>0.004097713321771002</v>
       </c>
       <c r="D276" s="1">
-        <v>0.09659799999999952</v>
+        <v>0.09659649999999931</v>
       </c>
     </row>
     <row r="277" spans="1:4">
-      <c r="A277" s="4">
+      <c r="A277" s="3">
         <v>38079</v>
       </c>
       <c r="B277">
-        <v>110203.47</v>
+        <v>110203.32</v>
       </c>
       <c r="C277" s="1">
-        <v>0.004957787630471611</v>
+        <v>0.004957794412074001</v>
       </c>
       <c r="D277" s="1">
-        <v>0.1020346999999995</v>
+        <v>0.1020331999999993</v>
       </c>
     </row>
     <row r="278" spans="1:4">
-      <c r="A278" s="4">
+      <c r="A278" s="3">
         <v>38080</v>
       </c>
       <c r="B278">
-        <v>110203.47</v>
+        <v>110203.32</v>
       </c>
       <c r="C278" s="1">
         <v>0</v>
       </c>
       <c r="D278" s="1">
-        <v>0.1020346999999995</v>
+        <v>0.1020331999999993</v>
       </c>
     </row>
     <row r="279" spans="1:4">
-      <c r="A279" s="4">
+      <c r="A279" s="3">
         <v>38081</v>
       </c>
       <c r="B279">
-        <v>110203.47</v>
+        <v>110203.32</v>
       </c>
       <c r="C279" s="1">
         <v>0</v>
       </c>
       <c r="D279" s="1">
-        <v>0.1020346999999995</v>
+        <v>0.1020331999999993</v>
       </c>
     </row>
     <row r="280" spans="1:4">
-      <c r="A280" s="4">
+      <c r="A280" s="3">
         <v>38082</v>
       </c>
       <c r="B280">
-        <v>110884.31</v>
+        <v>110884.16</v>
       </c>
       <c r="C280" s="1">
-        <v>0.006178026880641951</v>
+        <v>0.006178035289680972</v>
       </c>
       <c r="D280" s="1">
-        <v>0.1088430999999996</v>
+        <v>0.1088415999999992</v>
       </c>
     </row>
     <row r="281" spans="1:4">
-      <c r="A281" s="4">
+      <c r="A281" s="3">
         <v>38083</v>
       </c>
       <c r="B281">
-        <v>110875.43</v>
+        <v>110875.28</v>
       </c>
       <c r="C281" s="1">
-        <v>-8.008346717403025E-05</v>
+        <v>-8.008357550803868E-05</v>
       </c>
       <c r="D281" s="1">
-        <v>0.1087542999999997</v>
+        <v>0.1087527999999991</v>
       </c>
     </row>
     <row r="282" spans="1:4">
-      <c r="A282" s="4">
+      <c r="A282" s="3">
         <v>38084</v>
       </c>
       <c r="B282">
-        <v>110219.53</v>
+        <v>110219.38</v>
       </c>
       <c r="C282" s="1">
-        <v>-0.005915647858141249</v>
+        <v>-0.005915655861252311</v>
       </c>
       <c r="D282" s="1">
-        <v>0.1021952999999998</v>
+        <v>0.1021937999999991</v>
       </c>
     </row>
     <row r="283" spans="1:4">
-      <c r="A283" s="4">
+      <c r="A283" s="3">
         <v>38085</v>
       </c>
       <c r="B283">
-        <v>109830.5600000001</v>
+        <v>109831.84</v>
       </c>
       <c r="C283" s="1">
-        <v>-0.003529047891966064</v>
+        <v>-0.003516078569848591</v>
       </c>
       <c r="D283" s="1">
-        <v>0.09830559999999977</v>
+        <v>0.09831839999999903</v>
       </c>
     </row>
     <row r="284" spans="1:4">
-      <c r="A284" s="4">
+      <c r="A284" s="3">
         <v>38086</v>
       </c>
       <c r="B284">
-        <v>109830.5600000001</v>
+        <v>109831.84</v>
       </c>
       <c r="C284" s="1">
         <v>0</v>
       </c>
       <c r="D284" s="1">
-        <v>0.09830559999999977</v>
+        <v>0.09831839999999903</v>
       </c>
     </row>
     <row r="285" spans="1:4">
-      <c r="A285" s="4">
+      <c r="A285" s="3">
         <v>38087</v>
       </c>
       <c r="B285">
-        <v>109830.5600000001</v>
+        <v>109831.84</v>
       </c>
       <c r="C285" s="1">
         <v>0</v>
       </c>
       <c r="D285" s="1">
-        <v>0.09830559999999977</v>
+        <v>0.09831839999999903</v>
       </c>
     </row>
     <row r="286" spans="1:4">
-      <c r="A286" s="4">
+      <c r="A286" s="3">
         <v>38088</v>
       </c>
       <c r="B286">
-        <v>109830.5600000001</v>
+        <v>109831.84</v>
       </c>
       <c r="C286" s="1">
         <v>0</v>
       </c>
       <c r="D286" s="1">
-        <v>0.09830559999999977</v>
+        <v>0.09831839999999903</v>
       </c>
     </row>
     <row r="287" spans="1:4">
-      <c r="A287" s="4">
+      <c r="A287" s="3">
         <v>38089</v>
       </c>
       <c r="B287">
-        <v>109927.38</v>
+        <v>109938.25</v>
       </c>
       <c r="C287" s="1">
-        <v>0.0008815397098949074</v>
+        <v>0.0009688447357343311</v>
       </c>
       <c r="D287" s="1">
-        <v>0.09927379999999975</v>
+        <v>0.09938249999999926</v>
       </c>
     </row>
     <row r="288" spans="1:4">
-      <c r="A288" s="4">
+      <c r="A288" s="3">
         <v>38090</v>
       </c>
       <c r="B288">
-        <v>108644.56</v>
+        <v>108655.43</v>
       </c>
       <c r="C288" s="1">
-        <v>-0.01166970412648793</v>
+        <v>-0.0116685502998275</v>
       </c>
       <c r="D288" s="1">
-        <v>0.08644559999999957</v>
+        <v>0.08655429999999908</v>
       </c>
     </row>
     <row r="289" spans="1:4">
-      <c r="A289" s="4">
+      <c r="A289" s="3">
         <v>38091</v>
       </c>
       <c r="B289">
-        <v>108990.74</v>
+        <v>109001.61</v>
       </c>
       <c r="C289" s="1">
-        <v>0.003186353739202508</v>
+        <v>0.00318603497312564</v>
       </c>
       <c r="D289" s="1">
-        <v>0.08990739999999975</v>
+        <v>0.09001609999999904</v>
       </c>
     </row>
     <row r="290" spans="1:4">
-      <c r="A290" s="4">
+      <c r="A290" s="3">
         <v>38092</v>
       </c>
       <c r="B290">
-        <v>109868.5500000001</v>
+        <v>109879.4200000001</v>
       </c>
       <c r="C290" s="1">
-        <v>0.008053986971737315</v>
+        <v>0.008053183801597141</v>
       </c>
       <c r="D290" s="1">
-        <v>0.09868549999999976</v>
+        <v>0.09879419999999905</v>
       </c>
     </row>
     <row r="291" spans="1:4">
-      <c r="A291" s="4">
+      <c r="A291" s="3">
         <v>38093</v>
       </c>
       <c r="B291">
-        <v>110542.3100000001</v>
+        <v>110553.1800000001</v>
       </c>
       <c r="C291" s="1">
-        <v>0.006132419149974977</v>
+        <v>0.006131812490455468</v>
       </c>
       <c r="D291" s="1">
-        <v>0.1054230999999997</v>
+        <v>0.1055317999999992</v>
       </c>
     </row>
     <row r="292" spans="1:4">
-      <c r="A292" s="4">
+      <c r="A292" s="3">
         <v>38094</v>
       </c>
       <c r="B292">
-        <v>110542.3100000001</v>
+        <v>110553.1800000001</v>
       </c>
       <c r="C292" s="1">
         <v>0</v>
       </c>
       <c r="D292" s="1">
-        <v>0.1054230999999997</v>
+        <v>0.1055317999999992</v>
       </c>
     </row>
     <row r="293" spans="1:4">
-      <c r="A293" s="4">
+      <c r="A293" s="3">
         <v>38095</v>
       </c>
       <c r="B293">
-        <v>110542.3100000001</v>
+        <v>110553.1800000001</v>
       </c>
       <c r="C293" s="1">
         <v>0</v>
       </c>
       <c r="D293" s="1">
-        <v>0.1054230999999997</v>
+        <v>0.1055317999999992</v>
       </c>
     </row>
     <row r="294" spans="1:4">
-      <c r="A294" s="4">
+      <c r="A294" s="3">
         <v>38096</v>
       </c>
       <c r="B294">
-        <v>110525.8400000001</v>
+        <v>110536.7100000001</v>
       </c>
       <c r="C294" s="1">
-        <v>-0.0001489927250479806</v>
+        <v>-0.0001489780755289383</v>
       </c>
       <c r="D294" s="1">
-        <v>0.1052583999999996</v>
+        <v>0.1053670999999992</v>
       </c>
     </row>
     <row r="295" spans="1:4">
-      <c r="A295" s="4">
+      <c r="A295" s="3">
         <v>38097</v>
       </c>
       <c r="B295">
-        <v>109124.8700000001</v>
+        <v>109135.74</v>
       </c>
       <c r="C295" s="1">
-        <v>-0.01267549742214125</v>
+        <v>-0.0126742509343728</v>
       </c>
       <c r="D295" s="1">
-        <v>0.09124869999999974</v>
+        <v>0.09135739999999926</v>
       </c>
     </row>
     <row r="296" spans="1:4">
-      <c r="A296" s="4">
+      <c r="A296" s="3">
         <v>38098</v>
       </c>
       <c r="B296">
-        <v>109687.0900000001</v>
+        <v>109697.9600000001</v>
       </c>
       <c r="C296" s="1">
-        <v>0.00515207944806706</v>
+        <v>0.005151566297163512</v>
       </c>
       <c r="D296" s="1">
-        <v>0.09687089999999965</v>
+        <v>0.09697959999999917</v>
       </c>
     </row>
     <row r="297" spans="1:4">
-      <c r="A297" s="4">
+      <c r="A297" s="3">
         <v>38099</v>
       </c>
       <c r="B297">
-        <v>110790.0600000001</v>
+        <v>110800.9300000001</v>
       </c>
       <c r="C297" s="1">
-        <v>0.01005560453832799</v>
+        <v>0.01005460812580283</v>
       </c>
       <c r="D297" s="1">
-        <v>0.1079005999999996</v>
+        <v>0.1080092999999991</v>
       </c>
     </row>
     <row r="298" spans="1:4">
-      <c r="A298" s="4">
+      <c r="A298" s="3">
         <v>38100</v>
       </c>
       <c r="B298">
-        <v>110798.9100000001</v>
+        <v>110809.7800000001</v>
       </c>
       <c r="C298" s="1">
-        <v>7.988081241228073E-05</v>
+        <v>7.987297579536978E-05</v>
       </c>
       <c r="D298" s="1">
-        <v>0.1079890999999997</v>
+        <v>0.108097799999999</v>
       </c>
     </row>
     <row r="299" spans="1:4">
-      <c r="A299" s="4">
+      <c r="A299" s="3">
         <v>38101</v>
       </c>
       <c r="B299">
-        <v>110798.9100000001</v>
+        <v>110809.7800000001</v>
       </c>
       <c r="C299" s="1">
         <v>0</v>
       </c>
       <c r="D299" s="1">
-        <v>0.1079890999999997</v>
+        <v>0.108097799999999</v>
       </c>
     </row>
     <row r="300" spans="1:4">
-      <c r="A300" s="4">
+      <c r="A300" s="3">
         <v>38102</v>
       </c>
       <c r="B300">
-        <v>110798.9100000001</v>
+        <v>110809.7800000001</v>
       </c>
       <c r="C300" s="1">
         <v>0</v>
       </c>
       <c r="D300" s="1">
-        <v>0.1079890999999997</v>
+        <v>0.108097799999999</v>
       </c>
     </row>
     <row r="301" spans="1:4">
-      <c r="A301" s="4">
+      <c r="A301" s="3">
         <v>38103</v>
       </c>
       <c r="B301">
-        <v>110577.5100000001</v>
+        <v>110588.38</v>
       </c>
       <c r="C301" s="1">
-        <v>-0.001998214603374793</v>
+        <v>-0.001998018586446104</v>
       </c>
       <c r="D301" s="1">
-        <v>0.1057750999999996</v>
+        <v>0.1058837999999991</v>
       </c>
     </row>
     <row r="302" spans="1:4">
-      <c r="A302" s="4">
+      <c r="A302" s="3">
         <v>38104</v>
       </c>
       <c r="B302">
-        <v>110857.26</v>
+        <v>110868.13</v>
       </c>
       <c r="C302" s="1">
-        <v>0.002529899615210995</v>
+        <v>0.002529650945243933</v>
       </c>
       <c r="D302" s="1">
-        <v>0.1085725999999996</v>
+        <v>0.1086812999999991</v>
       </c>
     </row>
     <row r="303" spans="1:4">
-      <c r="A303" s="4">
+      <c r="A303" s="3">
         <v>38105</v>
       </c>
       <c r="B303">
-        <v>109854.6800000001</v>
+        <v>109865.55</v>
       </c>
       <c r="C303" s="1">
-        <v>-0.009043882195897579</v>
+        <v>-0.009042995493835693</v>
       </c>
       <c r="D303" s="1">
-        <v>0.0985467999999996</v>
+        <v>0.09865549999999912</v>
       </c>
     </row>
     <row r="304" spans="1:4">
-      <c r="A304" s="4">
+      <c r="A304" s="3">
         <v>38106</v>
       </c>
       <c r="B304">
-        <v>109360.7300000001</v>
+        <v>109371.6</v>
       </c>
       <c r="C304" s="1">
-        <v>-0.004496394691605232</v>
+        <v>-0.004495949822305501</v>
       </c>
       <c r="D304" s="1">
-        <v>0.09360729999999973</v>
+        <v>0.09371599999999924</v>
       </c>
     </row>
     <row r="305" spans="1:4">
-      <c r="A305" s="4">
+      <c r="A305" s="3">
         <v>38107</v>
       </c>
       <c r="B305">
-        <v>109183.24</v>
+        <v>109194.11</v>
       </c>
       <c r="C305" s="1">
-        <v>-0.001622977461836705</v>
+        <v>-0.00162281616068527</v>
       </c>
       <c r="D305" s="1">
-        <v>0.0918323999999997</v>
+        <v>0.09194109999999922</v>
       </c>
     </row>
     <row r="306" spans="1:4">
-      <c r="A306" s="4">
+      <c r="A306" s="3">
         <v>38108</v>
       </c>
       <c r="B306">
-        <v>109183.24</v>
+        <v>109194.11</v>
       </c>
       <c r="C306" s="1">
         <v>0</v>
       </c>
       <c r="D306" s="1">
-        <v>0.0918323999999997</v>
+        <v>0.09194109999999922</v>
       </c>
     </row>
     <row r="307" spans="1:4">
-      <c r="A307" s="4">
+      <c r="A307" s="3">
         <v>38109</v>
       </c>
       <c r="B307">
-        <v>109183.24</v>
+        <v>109194.11</v>
       </c>
       <c r="C307" s="1">
         <v>0</v>
       </c>
       <c r="D307" s="1">
-        <v>0.0918323999999997</v>
+        <v>0.09194109999999922</v>
       </c>
     </row>
     <row r="308" spans="1:4">
-      <c r="A308" s="4">
+      <c r="A308" s="3">
         <v>38110</v>
       </c>
       <c r="B308">
-        <v>110113.24</v>
+        <v>110124.11</v>
       </c>
       <c r="C308" s="1">
-        <v>0.008517790825771199</v>
+        <v>0.008516942901040991</v>
       </c>
       <c r="D308" s="1">
-        <v>0.1011323999999993</v>
+        <v>0.1012410999999991</v>
       </c>
     </row>
     <row r="309" spans="1:4">
-      <c r="A309" s="4">
+      <c r="A309" s="3">
         <v>38111</v>
       </c>
       <c r="B309">
-        <v>110119.29</v>
+        <v>110130.16</v>
       </c>
       <c r="C309" s="1">
-        <v>5.494343822776138E-05</v>
+        <v>5.493801493616779E-05</v>
       </c>
       <c r="D309" s="1">
-        <v>0.1011928999999994</v>
+        <v>0.1013015999999991</v>
       </c>
     </row>
     <row r="310" spans="1:4">
-      <c r="A310" s="4">
+      <c r="A310" s="3">
         <v>38112</v>
       </c>
       <c r="B310">
-        <v>110249.7200000001</v>
+        <v>110260.5900000001</v>
       </c>
       <c r="C310" s="1">
-        <v>0.001184442798350949</v>
+        <v>0.001184325892199078</v>
       </c>
       <c r="D310" s="1">
-        <v>0.1024971999999995</v>
+        <v>0.1026058999999995</v>
       </c>
     </row>
     <row r="311" spans="1:4">
-      <c r="A311" s="4">
+      <c r="A311" s="3">
         <v>38113</v>
       </c>
       <c r="B311">
-        <v>109936.4600000001</v>
+        <v>109947.3300000001</v>
       </c>
       <c r="C311" s="1">
-        <v>-0.002841367760389679</v>
+        <v>-0.002841087645186646</v>
       </c>
       <c r="D311" s="1">
-        <v>0.09936459999999969</v>
+        <v>0.09947329999999965</v>
       </c>
     </row>
     <row r="312" spans="1:4">
-      <c r="A312" s="4">
+      <c r="A312" s="3">
         <v>38114</v>
       </c>
       <c r="B312">
-        <v>108688.52</v>
+        <v>108699.39</v>
       </c>
       <c r="C312" s="1">
-        <v>-0.0113514661105153</v>
+        <v>-0.01135034384191058</v>
       </c>
       <c r="D312" s="1">
-        <v>0.08688519999999955</v>
+        <v>0.08699389999999951</v>
       </c>
     </row>
     <row r="313" spans="1:4">
-      <c r="A313" s="4">
+      <c r="A313" s="3">
         <v>38115</v>
       </c>
       <c r="B313">
-        <v>108688.52</v>
+        <v>108699.39</v>
       </c>
       <c r="C313" s="1">
         <v>0</v>
       </c>
       <c r="D313" s="1">
-        <v>0.08688519999999955</v>
+        <v>0.08699389999999951</v>
       </c>
     </row>
     <row r="314" spans="1:4">
-      <c r="A314" s="4">
+      <c r="A314" s="3">
         <v>38116</v>
       </c>
       <c r="B314">
-        <v>108688.52</v>
+        <v>108699.39</v>
       </c>
       <c r="C314" s="1">
         <v>0</v>
       </c>
       <c r="D314" s="1">
-        <v>0.08688519999999955</v>
+        <v>0.08699389999999951</v>
       </c>
     </row>
     <row r="315" spans="1:4">
-      <c r="A315" s="4">
+      <c r="A315" s="3">
         <v>38117</v>
       </c>
       <c r="B315">
-        <v>107617.2900000001</v>
+        <v>107628.16</v>
       </c>
       <c r="C315" s="1">
-        <v>-0.009855962708849031</v>
+        <v>-0.009854977107047191</v>
       </c>
       <c r="D315" s="1">
-        <v>0.07617289999999954</v>
+        <v>0.07628159999999951</v>
       </c>
     </row>
     <row r="316" spans="1:4">
-      <c r="A316" s="4">
+      <c r="A316" s="3">
         <v>38118</v>
       </c>
       <c r="B316">
-        <v>107831.3100000001</v>
+        <v>107842.1800000001</v>
       </c>
       <c r="C316" s="1">
-        <v>0.00198871389532318</v>
+        <v>0.001988513043426732</v>
       </c>
       <c r="D316" s="1">
-        <v>0.07831309999999969</v>
+        <v>0.07842179999999965</v>
       </c>
     </row>
     <row r="317" spans="1:4">
-      <c r="A317" s="4">
+      <c r="A317" s="3">
         <v>38119</v>
       </c>
       <c r="B317">
-        <v>107940.49</v>
+        <v>107951.36</v>
       </c>
       <c r="C317" s="1">
-        <v>0.001012507406243923</v>
+        <v>0.001012405350114154</v>
       </c>
       <c r="D317" s="1">
-        <v>0.07940489999999945</v>
+        <v>0.07951359999999941</v>
       </c>
     </row>
     <row r="318" spans="1:4">
-      <c r="A318" s="4">
+      <c r="A318" s="3">
         <v>38120</v>
       </c>
       <c r="B318">
-        <v>107809.02</v>
+        <v>107819.89</v>
       </c>
       <c r="C318" s="1">
-        <v>-0.001217985947627342</v>
+        <v>-0.001217863304362354</v>
       </c>
       <c r="D318" s="1">
-        <v>0.07809019999999944</v>
+        <v>0.0781988999999994</v>
       </c>
     </row>
     <row r="319" spans="1:4">
-      <c r="A319" s="4">
+      <c r="A319" s="3">
         <v>38121</v>
       </c>
       <c r="B319">
-        <v>108052.39</v>
+        <v>108063.26</v>
       </c>
       <c r="C319" s="1">
-        <v>0.002257417793056771</v>
+        <v>0.002257190208597049</v>
       </c>
       <c r="D319" s="1">
-        <v>0.08052389999999954</v>
+        <v>0.0806325999999995</v>
       </c>
     </row>
     <row r="320" spans="1:4">
-      <c r="A320" s="4">
+      <c r="A320" s="3">
         <v>38122</v>
       </c>
       <c r="B320">
-        <v>108052.39</v>
+        <v>108063.26</v>
       </c>
       <c r="C320" s="1">
         <v>0</v>
       </c>
       <c r="D320" s="1">
-        <v>0.08052389999999954</v>
+        <v>0.0806325999999995</v>
       </c>
     </row>
     <row r="321" spans="1:4">
-      <c r="A321" s="4">
+      <c r="A321" s="3">
         <v>38123</v>
       </c>
       <c r="B321">
-        <v>108052.39</v>
+        <v>108063.26</v>
       </c>
       <c r="C321" s="1">
         <v>0</v>
       </c>
       <c r="D321" s="1">
-        <v>0.08052389999999954</v>
+        <v>0.0806325999999995</v>
       </c>
     </row>
     <row r="322" spans="1:4">
-      <c r="A322" s="4">
+      <c r="A322" s="3">
         <v>38124</v>
       </c>
       <c r="B322">
-        <v>107263.7700000001</v>
+        <v>107274.6400000001</v>
       </c>
       <c r="C322" s="1">
-        <v>-0.007298496590403825</v>
+        <v>-0.00729776244025937</v>
       </c>
       <c r="D322" s="1">
-        <v>0.07263769999999981</v>
+        <v>0.07274639999999977</v>
       </c>
     </row>
     <row r="323" spans="1:4">
-      <c r="A323" s="4">
+      <c r="A323" s="3">
         <v>38125</v>
       </c>
       <c r="B323">
-        <v>107657.8200000001</v>
+        <v>107668.69</v>
       </c>
       <c r="C323" s="1">
-        <v>0.003673654207753341</v>
+        <v>0.003673281961141805</v>
       </c>
       <c r="D323" s="1">
-        <v>0.07657819999999971</v>
+        <v>0.07668689999999967</v>
       </c>
     </row>
     <row r="324" spans="1:4">
-      <c r="A324" s="4">
+      <c r="A324" s="3">
         <v>38126</v>
       </c>
       <c r="B324">
-        <v>107136.1000000001</v>
+        <v>107146.9700000001</v>
       </c>
       <c r="C324" s="1">
-        <v>-0.004846094784382471</v>
+        <v>-0.004845605533047581</v>
       </c>
       <c r="D324" s="1">
-        <v>0.07136099999999979</v>
+        <v>0.07146969999999975</v>
       </c>
     </row>
     <row r="325" spans="1:4">
-      <c r="A325" s="4">
+      <c r="A325" s="3">
         <v>38127</v>
       </c>
       <c r="B325">
-        <v>107110.45</v>
+        <v>107121.32</v>
       </c>
       <c r="C325" s="1">
-        <v>-0.0002394150991125166</v>
+        <v>-0.000239390810584994</v>
       </c>
       <c r="D325" s="1">
-        <v>0.07110449999999946</v>
+        <v>0.07121319999999942</v>
       </c>
     </row>
     <row r="326" spans="1:4">
-      <c r="A326" s="4">
+      <c r="A326" s="3">
         <v>38128</v>
       </c>
       <c r="B326">
-        <v>107302.1600000001</v>
+        <v>107313.0300000001</v>
       </c>
       <c r="C326" s="1">
-        <v>0.001789834698668891</v>
+        <v>0.00178965307746437</v>
       </c>
       <c r="D326" s="1">
-        <v>0.07302159999999991</v>
+        <v>0.07313029999999987</v>
       </c>
     </row>
     <row r="327" spans="1:4">
-      <c r="A327" s="4">
+      <c r="A327" s="3">
         <v>38129</v>
       </c>
       <c r="B327">
-        <v>107302.1600000001</v>
+        <v>107313.0300000001</v>
       </c>
       <c r="C327" s="1">
         <v>0</v>
       </c>
       <c r="D327" s="1">
-        <v>0.07302159999999991</v>
+        <v>0.07313029999999987</v>
       </c>
     </row>
     <row r="328" spans="1:4">
-      <c r="A328" s="4">
+      <c r="A328" s="3">
         <v>38130</v>
       </c>
       <c r="B328">
-        <v>107302.1600000001</v>
+        <v>107313.0300000001</v>
       </c>
       <c r="C328" s="1">
         <v>0</v>
       </c>
       <c r="D328" s="1">
-        <v>0.07302159999999991</v>
+        <v>0.07313029999999987</v>
       </c>
     </row>
     <row r="329" spans="1:4">
-      <c r="A329" s="4">
+      <c r="A329" s="3">
         <v>38131</v>
       </c>
       <c r="B329">
-        <v>107285.3500000001</v>
+        <v>107296.2200000001</v>
       </c>
       <c r="C329" s="1">
-        <v>-0.0001566604064635602</v>
+        <v>-0.0001566445379467263</v>
       </c>
       <c r="D329" s="1">
-        <v>0.07285349999999968</v>
+        <v>0.07296219999999964</v>
       </c>
     </row>
     <row r="330" spans="1:4">
-      <c r="A330" s="4">
+      <c r="A330" s="3">
         <v>38132</v>
       </c>
       <c r="B330">
-        <v>108635.58</v>
+        <v>108646.45</v>
       </c>
       <c r="C330" s="1">
-        <v>0.0125854089118409</v>
+        <v>0.01258413390518309</v>
       </c>
       <c r="D330" s="1">
-        <v>0.08635579999999932</v>
+        <v>0.0864644999999995</v>
       </c>
     </row>
     <row r="331" spans="1:4">
-      <c r="A331" s="4">
+      <c r="A331" s="3">
         <v>38133</v>
       </c>
       <c r="B331">
-        <v>108855.4000000001</v>
+        <v>108866.27</v>
       </c>
       <c r="C331" s="1">
-        <v>0.002023462294765688</v>
+        <v>0.002023259848803249</v>
       </c>
       <c r="D331" s="1">
-        <v>0.08855399999999936</v>
+        <v>0.08866269999999954</v>
       </c>
     </row>
     <row r="332" spans="1:4">
-      <c r="A332" s="4">
+      <c r="A332" s="3">
         <v>38134</v>
       </c>
       <c r="B332">
-        <v>109719.7100000001</v>
+        <v>109730.58</v>
       </c>
       <c r="C332" s="1">
-        <v>0.007939982766128173</v>
+        <v>0.007939189980514572</v>
       </c>
       <c r="D332" s="1">
-        <v>0.09719709999999915</v>
+        <v>0.09730579999999955</v>
       </c>
     </row>
     <row r="333" spans="1:4">
-      <c r="A333" s="4">
+      <c r="A333" s="3">
         <v>38135</v>
       </c>
       <c r="B333">
-        <v>109655.87</v>
+        <v>109666.74</v>
       </c>
       <c r="C333" s="1">
-        <v>-0.0005818462334616914</v>
+        <v>-0.0005817885953032231</v>
       </c>
       <c r="D333" s="1">
-        <v>0.096558699999999</v>
+        <v>0.0966673999999994</v>
       </c>
     </row>
     <row r="334" spans="1:4">
-      <c r="A334" s="4">
+      <c r="A334" s="3">
         <v>38136</v>
       </c>
       <c r="B334">
-        <v>109655.87</v>
+        <v>109666.74</v>
       </c>
       <c r="C334" s="1">
         <v>0</v>
       </c>
       <c r="D334" s="1">
-        <v>0.096558699999999</v>
+        <v>0.0966673999999994</v>
       </c>
     </row>
     <row r="335" spans="1:4">
-      <c r="A335" s="4">
+      <c r="A335" s="3">
         <v>38137</v>
       </c>
       <c r="B335">
-        <v>109655.87</v>
+        <v>109666.74</v>
       </c>
       <c r="C335" s="1">
         <v>0</v>
       </c>
       <c r="D335" s="1">
-        <v>0.096558699999999</v>
+        <v>0.0966673999999994</v>
       </c>
     </row>
     <row r="336" spans="1:4">
-      <c r="A336" s="4">
+      <c r="A336" s="3">
         <v>38138</v>
       </c>
       <c r="B336">
-        <v>109655.87</v>
+        <v>109666.74</v>
       </c>
       <c r="C336" s="1">
         <v>0</v>
       </c>
       <c r="D336" s="1">
-        <v>0.096558699999999</v>
+        <v>0.0966673999999994</v>
       </c>
     </row>
     <row r="337" spans="1:4">
-      <c r="A337" s="4">
+      <c r="A337" s="3">
         <v>38139</v>
       </c>
       <c r="B337">
-        <v>109849.5400000001</v>
+        <v>109860.41</v>
       </c>
       <c r="C337" s="1">
-        <v>0.00176616172029842</v>
+        <v>0.00176598666104244</v>
       </c>
       <c r="D337" s="1">
-        <v>0.09849539999999912</v>
+        <v>0.09860409999999953</v>
       </c>
     </row>
     <row r="338" spans="1:4">
-      <c r="A338" s="4">
+      <c r="A338" s="3">
         <v>38140</v>
       </c>
       <c r="B338">
-        <v>110277.9400000001</v>
+        <v>110288.8100000001</v>
       </c>
       <c r="C338" s="1">
-        <v>0.003899879781016802</v>
+        <v>0.003899493912320251</v>
       </c>
       <c r="D338" s="1">
-        <v>0.1027793999999991</v>
+        <v>0.1028880999999997</v>
       </c>
     </row>
     <row r="339" spans="1:4">
-      <c r="A339" s="4">
+      <c r="A339" s="3">
         <v>38141</v>
       </c>
       <c r="B339">
-        <v>109826.3300000001</v>
+        <v>109837.2000000001</v>
       </c>
       <c r="C339" s="1">
-        <v>-0.004095198006056178</v>
+        <v>-0.004094794385758549</v>
       </c>
       <c r="D339" s="1">
-        <v>0.09826329999999928</v>
+        <v>0.09837199999999968</v>
       </c>
     </row>
     <row r="340" spans="1:4">
-      <c r="A340" s="4">
+      <c r="A340" s="3">
         <v>38142</v>
       </c>
       <c r="B340">
-        <v>110142.7600000001</v>
+        <v>110153.6300000001</v>
       </c>
       <c r="C340" s="1">
-        <v>0.002881185231264682</v>
+        <v>0.002880900095778127</v>
       </c>
       <c r="D340" s="1">
-        <v>0.1014275999999994</v>
+        <v>0.1015362999999998</v>
       </c>
     </row>
     <row r="341" spans="1:4">
-      <c r="A341" s="4">
+      <c r="A341" s="3">
         <v>38143</v>
       </c>
       <c r="B341">
-        <v>110142.7600000001</v>
+        <v>110153.6300000001</v>
       </c>
       <c r="C341" s="1">
         <v>0</v>
       </c>
       <c r="D341" s="1">
-        <v>0.1014275999999994</v>
+        <v>0.1015362999999998</v>
       </c>
     </row>
     <row r="342" spans="1:4">
-      <c r="A342" s="4">
+      <c r="A342" s="3">
         <v>38144</v>
       </c>
       <c r="B342">
-        <v>110142.7600000001</v>
+        <v>110153.6300000001</v>
       </c>
       <c r="C342" s="1">
         <v>0</v>
       </c>
       <c r="D342" s="1">
-        <v>0.1014275999999994</v>
+        <v>0.1015362999999998</v>
       </c>
     </row>
     <row r="343" spans="1:4">
-      <c r="A343" s="4">
+      <c r="A343" s="3">
         <v>38145</v>
       </c>
       <c r="B343">
-        <v>111245.1100000001</v>
+        <v>111255.9800000001</v>
       </c>
       <c r="C343" s="1">
-        <v>0.01000837458585568</v>
+        <v>0.01000738695583614</v>
       </c>
       <c r="D343" s="1">
-        <v>0.1124510999999995</v>
+        <v>0.1125597999999999</v>
       </c>
     </row>
     <row r="344" spans="1:4">
-      <c r="A344" s="4">
+      <c r="A344" s="3">
         <v>38146</v>
       </c>
       <c r="B344">
-        <v>111398.1200000001</v>
+        <v>111408.9900000001</v>
       </c>
       <c r="C344" s="1">
-        <v>0.001375431243674452</v>
+        <v>0.001375296860447461</v>
       </c>
       <c r="D344" s="1">
-        <v>0.1139811999999996</v>
+        <v>0.1140899</v>
       </c>
     </row>
     <row r="345" spans="1:4">
-      <c r="A345" s="4">
+      <c r="A345" s="3">
         <v>38147</v>
       </c>
       <c r="B345">
-        <v>110594.8900000001</v>
+        <v>110605.7600000001</v>
       </c>
       <c r="C345" s="1">
-        <v>-0.007210444844132136</v>
+        <v>-0.007209741332364739</v>
       </c>
       <c r="D345" s="1">
-        <v>0.1059488999999993</v>
+        <v>0.1060576</v>
       </c>
     </row>
     <row r="346" spans="1:4">
-      <c r="A346" s="4">
+      <c r="A346" s="3">
         <v>38148</v>
       </c>
       <c r="B346">
-        <v>110809.1500000001</v>
+        <v>110820.0200000001</v>
       </c>
       <c r="C346" s="1">
-        <v>0.001937340866291493</v>
+        <v>0.001937150470282978</v>
       </c>
       <c r="D346" s="1">
-        <v>0.1080914999999996</v>
+        <v>0.1082002</v>
       </c>
     </row>
     <row r="347" spans="1:4">
-      <c r="A347" s="4">
+      <c r="A347" s="3">
         <v>38149</v>
       </c>
       <c r="B347">
-        <v>110809.1500000001</v>
+        <v>110820.0200000001</v>
       </c>
       <c r="C347" s="1">
         <v>0</v>
       </c>
       <c r="D347" s="1">
-        <v>0.1080914999999996</v>
+        <v>0.1082002</v>
       </c>
     </row>
     <row r="348" spans="1:4">
-      <c r="A348" s="4">
+      <c r="A348" s="3">
         <v>38150</v>
       </c>
       <c r="B348">
-        <v>110809.1500000001</v>
+        <v>110820.0200000001</v>
       </c>
       <c r="C348" s="1">
         <v>0</v>
       </c>
       <c r="D348" s="1">
-        <v>0.1080914999999996</v>
+        <v>0.1082002</v>
       </c>
     </row>
     <row r="349" spans="1:4">
-      <c r="A349" s="4">
+      <c r="A349" s="3">
         <v>38151</v>
       </c>
       <c r="B349">
-        <v>110809.1500000001</v>
+        <v>110820.0200000001</v>
       </c>
       <c r="C349" s="1">
         <v>0</v>
       </c>
       <c r="D349" s="1">
-        <v>0.1080914999999996</v>
+        <v>0.1082002</v>
       </c>
     </row>
     <row r="350" spans="1:4">
-      <c r="A350" s="4">
+      <c r="A350" s="3">
         <v>38152</v>
       </c>
       <c r="B350">
-        <v>110145.2600000001</v>
+        <v>110156.1300000001</v>
       </c>
       <c r="C350" s="1">
-        <v>-0.005991292235343226</v>
+        <v>-0.005990704567640281</v>
       </c>
       <c r="D350" s="1">
-        <v>0.1014525999999998</v>
+        <v>0.1015613000000002</v>
       </c>
     </row>
     <row r="351" spans="1:4">
-      <c r="A351" s="4">
+      <c r="A351" s="3">
         <v>38153</v>
       </c>
       <c r="B351">
-        <v>110496.1800000001</v>
+        <v>110507.0500000001</v>
       </c>
       <c r="C351" s="1">
-        <v>0.003185974593913343</v>
+        <v>0.003185660207924768</v>
       </c>
       <c r="D351" s="1">
-        <v>0.1049617999999997</v>
+        <v>0.1050705000000001</v>
       </c>
     </row>
     <row r="352" spans="1:4">
-      <c r="A352" s="4">
+      <c r="A352" s="3">
         <v>38154</v>
       </c>
       <c r="B352">
-        <v>110591.9500000001</v>
+        <v>110602.8200000001</v>
       </c>
       <c r="C352" s="1">
-        <v>0.0008667267954423075</v>
+        <v>0.000866641540064883</v>
       </c>
       <c r="D352" s="1">
-        <v>0.1059194999999997</v>
+        <v>0.1060282000000003</v>
       </c>
     </row>
     <row r="353" spans="1:4">
-      <c r="A353" s="4">
+      <c r="A353" s="3">
         <v>38155</v>
       </c>
       <c r="B353">
-        <v>110486.7500000001</v>
+        <v>110497.6200000001</v>
       </c>
       <c r="C353" s="1">
-        <v>-0.0009512446430325339</v>
+        <v>-0.0009511511550973628</v>
       </c>
       <c r="D353" s="1">
-        <v>0.1048674999999994</v>
+        <v>0.1049762000000001</v>
       </c>
     </row>
     <row r="354" spans="1:4">
-      <c r="A354" s="4">
+      <c r="A354" s="3">
         <v>38156</v>
       </c>
       <c r="B354">
-        <v>110611.6600000001</v>
+        <v>110622.5300000001</v>
       </c>
       <c r="C354" s="1">
-        <v>0.001130542802643797</v>
+        <v>0.001130431587576197</v>
       </c>
       <c r="D354" s="1">
-        <v>0.1061165999999996</v>
+        <v>0.1062253</v>
       </c>
     </row>
     <row r="355" spans="1:4">
-      <c r="A355" s="4">
+      <c r="A355" s="3">
         <v>38157</v>
       </c>
       <c r="B355">
-        <v>110611.6600000001</v>
+        <v>110622.5300000001</v>
       </c>
       <c r="C355" s="1">
         <v>0</v>
       </c>
       <c r="D355" s="1">
-        <v>0.1061165999999996</v>
+        <v>0.1062253</v>
       </c>
     </row>
     <row r="356" spans="1:4">
-      <c r="A356" s="4">
+      <c r="A356" s="3">
         <v>38158</v>
       </c>
       <c r="B356">
-        <v>110611.6600000001</v>
+        <v>110622.5300000001</v>
       </c>
       <c r="C356" s="1">
         <v>0</v>
       </c>
       <c r="D356" s="1">
-        <v>0.1061165999999996</v>
+        <v>0.1062253</v>
       </c>
     </row>
     <row r="357" spans="1:4">
-      <c r="A357" s="4">
+      <c r="A357" s="3">
         <v>38159</v>
       </c>
       <c r="B357">
-        <v>110289.5500000001</v>
+        <v>110300.4200000001</v>
       </c>
       <c r="C357" s="1">
-        <v>-0.002912079974208837</v>
+        <v>-0.002911793827170661</v>
       </c>
       <c r="D357" s="1">
-        <v>0.1028954999999996</v>
+        <v>0.1030042</v>
       </c>
     </row>
     <row r="358" spans="1:4">
-      <c r="A358" s="4">
+      <c r="A358" s="3">
         <v>38160</v>
       </c>
       <c r="B358">
-        <v>110381.0500000001</v>
+        <v>110391.9200000001</v>
       </c>
       <c r="C358" s="1">
-        <v>0.0008296343579241583</v>
+        <v>0.000829552598258454</v>
       </c>
       <c r="D358" s="1">
-        <v>0.1038104999999996</v>
+        <v>0.1039192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>